<commit_message>
Reduced number of items in study
I have brought it down to only 10 descriptions and 10 images in the pre test. Also made it so that none of the descriptions have corresponding images in the pre-test. The post test has 25 images, some of which were only described in the pre-test, some which were shown in the pre-test, and some that did not show up at all previously in the study.
</commit_message>
<xml_diff>
--- a/Study Images/Image Usage.xlsx
+++ b/Study Images/Image Usage.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74e605293b3fb42f/SCHOOL/Spring 2018/Experimental Projects in Cognitive Science/Study/Study Images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\SCHOOL\Spring 2018\Experimental Projects in Cognitive Science\Study\Study Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="141" documentId="07C82EF4FF10AFC5914E076F47C4922DE320E31F" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{0141D887-8247-4DC4-958D-66B0905E8124}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{1CA9AEFD-D91A-4FD2-B1AD-C13427F6E3F9}"/>
   </bookViews>
@@ -415,15 +416,15 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>0</v>
       </c>
@@ -431,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -443,120 +444,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>SUM(A1:A70)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <f>SUM(B1:B70)</f>
-        <v>30</v>
+        <f>SUM(B1:B70) + SUM(A1:A70)</f>
+        <v>20</v>
       </c>
       <c r="G2">
         <f>SUM(C1:C70)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -565,51 +566,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>0</v>
       </c>
@@ -617,21 +618,21 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>0</v>
       </c>
@@ -639,21 +640,21 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>0</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>1</v>
       </c>
@@ -661,21 +662,21 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>0</v>
       </c>
@@ -683,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>0</v>
       </c>
@@ -697,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>0</v>
       </c>
@@ -705,21 +706,21 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>0</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>1</v>
       </c>
@@ -727,10 +728,10 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>0</v>
       </c>
@@ -738,10 +739,10 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>0</v>
       </c>
@@ -749,32 +750,32 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>0</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>0</v>
       </c>
@@ -782,10 +783,10 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>0</v>
       </c>
@@ -793,21 +794,21 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>0</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>0</v>
       </c>
@@ -815,21 +816,21 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>0</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>0</v>
       </c>
@@ -840,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>0</v>
       </c>
@@ -848,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>0</v>
       </c>
@@ -859,21 +860,21 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>0</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>0</v>
       </c>
@@ -881,10 +882,10 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>0</v>
       </c>
@@ -892,32 +893,32 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>0</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>0</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>0</v>
       </c>
@@ -925,43 +926,43 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>0</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>0</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>0</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>0</v>
       </c>
@@ -969,10 +970,10 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>0</v>
       </c>
@@ -980,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>0</v>
       </c>
@@ -994,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>0</v>
       </c>
@@ -1002,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>0</v>
       </c>
@@ -1013,21 +1014,21 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>0</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>0</v>
       </c>
@@ -1038,18 +1039,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>0</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>0</v>
       </c>
@@ -1057,21 +1058,21 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>0</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>0</v>
       </c>
@@ -1079,43 +1080,43 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>0</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>0</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>0</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>0</v>
       </c>
@@ -1123,10 +1124,10 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>0</v>
       </c>
@@ -1134,10 +1135,10 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>0</v>
       </c>
@@ -1145,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>0</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>0</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>0</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>0</v>
       </c>
@@ -1189,29 +1190,29 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>0</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>0</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>